<commit_message>
Output updates of Job2
</commit_message>
<xml_diff>
--- a/output/job2-Chart.xlsx
+++ b/output/job2-Chart.xlsx
@@ -173,11 +173,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -196,11 +197,19 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -386,6 +395,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -701,11 +711,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="88572873"/>
-        <c:axId val="34949195"/>
+        <c:axId val="62513568"/>
+        <c:axId val="33971603"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88572873"/>
+        <c:axId val="62513568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -778,14 +788,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34949195"/>
+        <c:crossAx val="33971603"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34949195"/>
+        <c:axId val="33971603"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +848,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -867,7 +877,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88572873"/>
+        <c:crossAx val="62513568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -956,6 +966,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1128,13 +1139,13 @@
                   <c:v>0.00181653042688465</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00435506596644037</c:v>
+                  <c:v>0.00409888561547329</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.000696985537550096</c:v>
+                  <c:v>0.000662136260672591</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1146,10 +1157,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.000936978362886208</c:v>
+                  <c:v>0.000897609524109477</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.000989948218093207</c:v>
+                  <c:v>0.000761498629302467</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1161,7 +1172,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.00206913613566336</c:v>
+                  <c:v>0.00204664552549311</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5.47006053533659E-005</c:v>
@@ -1170,7 +1181,7 @@
                   <c:v>0.00512163892445583</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.00192840785826202</c:v>
+                  <c:v>0.00180788236712065</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.000495540138751239</c:v>
@@ -1245,7 +1256,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0110098432373314</c:v>
+                  <c:v>0.00962449872402479</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0.00019358835372464</c:v>
@@ -1257,7 +1268,7 @@
                   <c:v>0.00363342753330642</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.000983131728307766</c:v>
+                  <c:v>0.000945318969526698</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>0.00217443827011355</c:v>
@@ -1271,11 +1282,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="5572384"/>
-        <c:axId val="40312549"/>
+        <c:axId val="41157176"/>
+        <c:axId val="36984303"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="5572384"/>
+        <c:axId val="41157176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,14 +1359,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40312549"/>
+        <c:crossAx val="36984303"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40312549"/>
+        <c:axId val="36984303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1419,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1437,7 +1448,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5572384"/>
+        <c:crossAx val="41157176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1475,9 +1486,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>170280</xdr:colOff>
+      <xdr:colOff>169920</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1485,8 +1496,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6050880" y="66960"/>
-        <a:ext cx="12259800" cy="5833080"/>
+        <a:off x="5959800" y="66960"/>
+        <a:ext cx="12069360" cy="5832720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1505,9 +1516,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>378000</xdr:colOff>
+      <xdr:colOff>377640</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1515,8 +1526,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6070680" y="6177240"/>
-        <a:ext cx="12447720" cy="4743000"/>
+        <a:off x="5979600" y="6177240"/>
+        <a:ext cx="12257280" cy="4742640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1536,16 +1547,16 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,7 +1589,7 @@
         <v>7807</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.00435506596644037</v>
+        <v>0.00409888561547329</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,7 +1611,7 @@
         <v>28695</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.000696985537550096</v>
+        <v>0.000662136260672591</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1655,7 @@
         <v>127004</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.000936978362886208</v>
+        <v>0.000897609524109477</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1666,7 @@
         <v>13132</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>0.000989948218093207</v>
+        <v>0.000761498629302467</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,7 +1710,7 @@
         <v>44463</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0.00206913613566336</v>
+        <v>0.00204664552549311</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,7 +1743,7 @@
         <v>8297</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>0.00192840785826202</v>
+        <v>0.00180788236712065</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,7 +2018,7 @@
         <v>13715</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>0.0110098432373314</v>
+        <v>0.00962449872402479</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,7 +2062,7 @@
         <v>793383</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>0.000983131728307766</v>
+        <v>0.000945318969526698</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>